<commit_message>
Modifica interfaz de cartera_operaciones, crea interfaz de rectificaciones
</commit_message>
<xml_diff>
--- a/Analisis/Interfaces/interfaces.xlsx
+++ b/Analisis/Interfaces/interfaces.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/Analisis/Interfaces/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="318" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04D9DF90-A5A9-492A-B071-249E29E94D4F}"/>
+  <xr:revisionPtr revIDLastSave="442" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFED54A1-64AB-4546-91FD-77EB8CDD5840}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resumen" sheetId="2" r:id="rId1"/>
     <sheet name="cartera_operaciones" sheetId="1" r:id="rId2"/>
     <sheet name="cuadro_operaciones" sheetId="5" r:id="rId3"/>
     <sheet name="tipo_cambio" sheetId="4" r:id="rId4"/>
+    <sheet name="cuadro_rectificaciones" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="114">
   <si>
     <t>Campo</t>
   </si>
@@ -487,6 +488,215 @@
       <t>1: Si
 2: NO</t>
     </r>
+  </si>
+  <si>
+    <t>Esta fecha de proceso corresponde a la fecha en que sera rectificado el archivo</t>
+  </si>
+  <si>
+    <t>fecha_a_rectificar</t>
+  </si>
+  <si>
+    <t>Corresponde a la fecha de proceso que se requiere rectificar</t>
+  </si>
+  <si>
+    <t>REDEC02</t>
+  </si>
+  <si>
+    <t>operación_desfasada</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Reportar 1 o 2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>1: Si es una operación desfasada
+2: NO es una operación desfasada</t>
+    </r>
+  </si>
+  <si>
+    <t>RDC01</t>
+  </si>
+  <si>
+    <t>RDC02</t>
+  </si>
+  <si>
+    <t>fecha_rectificacion</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Este campo tiene propositos de rectificacion, es decir, en el caso que la entidad no reporto una operación en una fecha particular.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>Solo para causal 2 en campo 30 RDC02 "Agregacion desfasada de la operación al registro"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Corresponde a la fecha de proceso donde se debio enviar esta informacion
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>Solo para causal 2 en campo 30 RDC02 "Agregacion desfasada de la operación al registro"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Corresponde a la fecha (AAAAMMDD) en que fue rectificada la operación en los sistemas internos del reportante.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>Solo para causal 2 en campo 30 RDC02 "Agregacion desfasada de la operación al registro"</t>
+    </r>
+  </si>
+  <si>
+    <t>causal_rectificacion</t>
+  </si>
+  <si>
+    <t>Default enviar vacío o 19000101
+Este campo solo se tomara en cuenta si en campo operación_desfasada se informa 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>Si aplica enviar 1,2,3,4,o 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t xml:space="preserve">
+Si no aplica enviar vacío
+Este campo solo se tomara en cuenta si en campo operación_desfasada se informa 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Se deberá completar el código considerando la causal de la rectificación de la siguiente tabla:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>1: Por errores u omisiones identificados internamente, sin previa solicitud del deudor.
+2: Por acoger totalmente una solicitud del deudor distinta a la del código 5.
+3: Por acoger parcialmente una solicitud del deudor.
+4: Por instrucción de la Comisión, tras rechazo de la solicitud por parte del reportante.
+5: Por acoger una solicitud del deudor relacionada a prescripción o liquidación concursal de la operación resuelta por un Tribunal.</t>
+    </r>
+  </si>
+  <si>
+    <t>numero_solicitud</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">En este campo se debe informar el código remitido en el campo NÚMERO DE LA SOLICITUD del archivo RDC40, cuando corresponda a causales por solicitud realizada por el deudor. Para ello se debe indicar el código remitido en el campo NÚMERO DE LA SOLICITUD del archivo RDC40. En dicho caso, el valor informado en el campo EVENTO de esta solicitud debe corresponder a cerrado (código 3) y el valor informado en el campo RESPUESTA DE LA SOLICITUD debe corresponder a acoge parcialmente (código 2) o acoge totalmente (código 1) la solicitud en el archivo RDC40.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>En los casos en que el campo 32 CAUSAL DE RECTIFICACIÓN se informe con códigos 1 o 4, se debe completar con blancos (espacios).</t>
+    </r>
+  </si>
+  <si>
+    <t>Solo se debe enviar si en el campo causal_rectificacion se informa 2,3 o 5
+Default vacío</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Causal de eliminacion, para esta interfaz solo se aceptan para los casos:
+1: Eliminacion de la operación
+0: Otro tipo de modificacion
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>Nota: Para agregacion se informa en la interfaz cartera_operaciones</t>
+    </r>
+  </si>
+  <si>
+    <t>Informar 1 o 0</t>
+  </si>
+  <si>
+    <t>campo_rdc01</t>
+  </si>
+  <si>
+    <t>Reportar el numero de campo a rectificar, si se requieren modificar mas campos, solo se deben enviar tantos registros en esta interface como campos se requieran modificar</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Informar el numero del campo del RDC01 que se requiere rectificar
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>Numeros del 1 al 28</t>
+    </r>
+  </si>
+  <si>
+    <t>En este campo se informara el valor a modificar.
+Si se requiere informar montos, se debera informar convertidos a pesos.</t>
+  </si>
+  <si>
+    <t>Informar con el formato que se requiere para el archivo, es decir, si el campo a modificar es fecha, reportar YYYYMMDD, si es un monto, informar en pesos</t>
+  </si>
+  <si>
+    <t>causal_eliminacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corresponde a la fecha (AAAAMMDD) en que fue rectificada la operación en los sistemas internos del reportante.
+</t>
   </si>
 </sst>
 </file>
@@ -533,7 +743,7 @@
       <name val="SimSun"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -543,6 +753,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -559,7 +775,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -610,6 +826,39 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -626,10 +875,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -912,24 +1157,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F22" sqref="A22:F22"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62" style="6" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="74.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="25.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="7"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="7" width="9.140625" style="7"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -946,10 +1191,13 @@
         <v>10</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>92</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
         <v>56</v>
       </c>
@@ -959,8 +1207,14 @@
       <c r="D2" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="48" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>4</v>
       </c>
@@ -976,8 +1230,11 @@
       <c r="F3" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="168" x14ac:dyDescent="0.15">
+      <c r="G3" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="144" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
         <v>8</v>
       </c>
@@ -996,8 +1253,11 @@
       <c r="F4" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+      <c r="G4" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
         <v>11</v>
       </c>
@@ -1010,8 +1270,11 @@
       <c r="F5" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="156" x14ac:dyDescent="0.15">
+      <c r="G5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="144" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
         <v>14</v>
       </c>
@@ -1030,8 +1293,11 @@
       <c r="F6" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="132" x14ac:dyDescent="0.15">
+      <c r="G6" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="132" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
         <v>17</v>
       </c>
@@ -1050,8 +1316,11 @@
       <c r="F7" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="72" x14ac:dyDescent="0.15">
+      <c r="G7" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
         <v>23</v>
       </c>
@@ -1070,8 +1339,11 @@
       <c r="F8" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="G8" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="24" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
         <v>27</v>
       </c>
@@ -1084,8 +1356,11 @@
       <c r="F9" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="276" x14ac:dyDescent="0.15">
+      <c r="G9" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="228" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
         <v>30</v>
       </c>
@@ -1102,8 +1377,11 @@
       <c r="F10" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="132" x14ac:dyDescent="0.15">
+      <c r="G10" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="96" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
         <v>34</v>
       </c>
@@ -1116,8 +1394,11 @@
       <c r="F11" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="252" x14ac:dyDescent="0.15">
+      <c r="G11" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="216" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
         <v>38</v>
       </c>
@@ -1130,8 +1411,11 @@
       <c r="F12" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="324" x14ac:dyDescent="0.15">
+      <c r="G12" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="276" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
         <v>40</v>
       </c>
@@ -1144,8 +1428,11 @@
       <c r="F13" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="72" x14ac:dyDescent="0.15">
+      <c r="G13" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
         <v>42</v>
       </c>
@@ -1158,8 +1445,11 @@
       <c r="F14" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="96" x14ac:dyDescent="0.15">
+      <c r="G14" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="84" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
         <v>44</v>
       </c>
@@ -1172,8 +1462,11 @@
       <c r="F15" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="120" x14ac:dyDescent="0.15">
+      <c r="G15" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="96" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
         <v>46</v>
       </c>
@@ -1189,8 +1482,11 @@
       <c r="F16" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+      <c r="G16" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="36" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
         <v>49</v>
       </c>
@@ -1206,8 +1502,11 @@
       <c r="F17" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+      <c r="G17" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="36" x14ac:dyDescent="0.15">
       <c r="A18" s="17" t="s">
         <v>50</v>
       </c>
@@ -1223,8 +1522,11 @@
       <c r="F18" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="G18" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="24" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
         <v>52</v>
       </c>
@@ -1240,8 +1542,11 @@
       <c r="F19" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="G19" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="24" x14ac:dyDescent="0.15">
       <c r="A20" s="17" t="s">
         <v>57</v>
       </c>
@@ -1254,8 +1559,11 @@
       <c r="F20" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="G20" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="24" x14ac:dyDescent="0.15">
       <c r="A21" s="17" t="s">
         <v>80</v>
       </c>
@@ -1271,8 +1579,11 @@
       <c r="F21" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="48" x14ac:dyDescent="0.15">
+      <c r="G21" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="36" x14ac:dyDescent="0.15">
       <c r="A22" s="17" t="s">
         <v>83</v>
       </c>
@@ -1286,6 +1597,104 @@
         <v>6</v>
       </c>
       <c r="F22" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="48" x14ac:dyDescent="0.15">
+      <c r="A23" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="22"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="48" x14ac:dyDescent="0.15">
+      <c r="A24" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="22"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="48" x14ac:dyDescent="0.15">
+      <c r="A25" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="22"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="144" x14ac:dyDescent="0.15">
+      <c r="A26" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="22"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="144" x14ac:dyDescent="0.15">
+      <c r="A27" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="22"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1299,7 +1708,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="A4:F4"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1347,7 +1756,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="15" t="s">
         <v>11</v>
       </c>
@@ -1557,4 +1966,197 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30384B7-8E23-4C8B-825F-E2F77541013E}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="7"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.15">
+      <c r="A2" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.15">
+      <c r="A3" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.15">
+      <c r="A4" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="84" x14ac:dyDescent="0.15">
+      <c r="A5" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="36" x14ac:dyDescent="0.15">
+      <c r="A6" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.15">
+      <c r="A7" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="36" x14ac:dyDescent="0.15">
+      <c r="A8" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="27"/>
+      <c r="D8" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="28"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="144" x14ac:dyDescent="0.15">
+      <c r="A9" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="28"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="144" x14ac:dyDescent="0.15">
+      <c r="A10" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="28"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Avance de creacion de schemas y tablas para interfaces
</commit_message>
<xml_diff>
--- a/Analisis/Interfaces/interfaces.xlsx
+++ b/Analisis/Interfaces/interfaces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/Analisis/Interfaces/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="442" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFED54A1-64AB-4546-91FD-77EB8CDD5840}"/>
+  <xr:revisionPtr revIDLastSave="453" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30857D36-F44A-4CB9-BA74-960D0B4FB221}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resumen" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="118">
   <si>
     <t>Campo</t>
   </si>
@@ -697,6 +697,18 @@
   <si>
     <t xml:space="preserve">Corresponde a la fecha (AAAAMMDD) en que fue rectificada la operación en los sistemas internos del reportante.
 </t>
+  </si>
+  <si>
+    <t>valor_contable</t>
+  </si>
+  <si>
+    <t>RDC22</t>
+  </si>
+  <si>
+    <t>Informar en moneda en pesos chilenos</t>
+  </si>
+  <si>
+    <t>Corresponde al valor de la cuenta contable reportada expresado por su equivalente en pesos a la fecha de referencia del archivo, cuando se trate de operaciones reajustables o en moneda extranjera.</t>
   </si>
 </sst>
 </file>
@@ -775,7 +787,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -845,21 +857,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -875,6 +872,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1146,9 +1147,9 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1157,24 +1158,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="7"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="22.44140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.109375" style="7"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1196,8 +1197,11 @@
       <c r="G1" s="12" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.15">
+      <c r="H1" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
         <v>56</v>
       </c>
@@ -1213,8 +1217,11 @@
       <c r="G2" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="48" x14ac:dyDescent="0.15">
+      <c r="H2" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="48" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>4</v>
       </c>
@@ -1234,7 +1241,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="144" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="144" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
         <v>8</v>
       </c>
@@ -1257,7 +1264,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
         <v>11</v>
       </c>
@@ -1274,7 +1281,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="144" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="144" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
         <v>14</v>
       </c>
@@ -1297,7 +1304,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="132" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="132" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
         <v>17</v>
       </c>
@@ -1320,7 +1327,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
         <v>23</v>
       </c>
@@ -1342,8 +1349,11 @@
       <c r="G8" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="24" x14ac:dyDescent="0.15">
+      <c r="H8" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
         <v>27</v>
       </c>
@@ -1360,7 +1370,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="228" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="228" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
         <v>30</v>
       </c>
@@ -1380,8 +1390,9 @@
       <c r="G10" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="96" x14ac:dyDescent="0.15">
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" ht="96" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
         <v>34</v>
       </c>
@@ -1398,7 +1409,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="216" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="216" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
         <v>38</v>
       </c>
@@ -1415,7 +1426,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="276" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="276" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
         <v>40</v>
       </c>
@@ -1432,7 +1443,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
         <v>42</v>
       </c>
@@ -1449,7 +1460,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="84" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="84" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
         <v>44</v>
       </c>
@@ -1466,7 +1477,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="96" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" ht="96" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
         <v>46</v>
       </c>
@@ -1486,7 +1497,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="36" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" ht="36" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
         <v>49</v>
       </c>
@@ -1506,7 +1517,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="36" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" ht="36" x14ac:dyDescent="0.15">
       <c r="A18" s="17" t="s">
         <v>50</v>
       </c>
@@ -1526,7 +1537,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="24" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
         <v>52</v>
       </c>
@@ -1546,7 +1557,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="24" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A20" s="17" t="s">
         <v>57</v>
       </c>
@@ -1563,7 +1574,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="24" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A21" s="17" t="s">
         <v>80</v>
       </c>
@@ -1583,7 +1594,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="36" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" ht="36" x14ac:dyDescent="0.15">
       <c r="A22" s="17" t="s">
         <v>83</v>
       </c>
@@ -1603,7 +1614,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="48" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" ht="48" x14ac:dyDescent="0.15">
       <c r="A23" s="19" t="s">
         <v>90</v>
       </c>
@@ -1621,8 +1632,9 @@
       <c r="G23" s="23" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="48" x14ac:dyDescent="0.15">
+      <c r="H23" s="23"/>
+    </row>
+    <row r="24" spans="1:8" ht="48" x14ac:dyDescent="0.15">
       <c r="A24" s="19" t="s">
         <v>87</v>
       </c>
@@ -1640,8 +1652,9 @@
       <c r="G24" s="23" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="48" x14ac:dyDescent="0.15">
+      <c r="H24" s="23"/>
+    </row>
+    <row r="25" spans="1:8" ht="48" x14ac:dyDescent="0.15">
       <c r="A25" s="19" t="s">
         <v>94</v>
       </c>
@@ -1659,8 +1672,9 @@
       <c r="G25" s="23" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="144" x14ac:dyDescent="0.15">
+      <c r="H25" s="23"/>
+    </row>
+    <row r="26" spans="1:8" ht="144" x14ac:dyDescent="0.15">
       <c r="A26" s="19" t="s">
         <v>98</v>
       </c>
@@ -1671,15 +1685,16 @@
         <v>100</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="23"/>
       <c r="G26" s="23" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="144" x14ac:dyDescent="0.15">
+      <c r="H26" s="23"/>
+    </row>
+    <row r="27" spans="1:8" ht="144" x14ac:dyDescent="0.15">
       <c r="A27" s="19" t="s">
         <v>102</v>
       </c>
@@ -1695,6 +1710,24 @@
       <c r="E27" s="22"/>
       <c r="F27" s="23"/>
       <c r="G27" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" s="23"/>
+    </row>
+    <row r="28" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H28" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1711,15 +1744,15 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.5703125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="7"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="22.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="7"/>
+    <col min="7" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -1901,14 +1934,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.15">
@@ -1972,19 +2005,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30384B7-8E23-4C8B-825F-E2F77541013E}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.5703125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="7"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="22.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.109375" style="7"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.15">
@@ -2024,7 +2057,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>87</v>
       </c>
@@ -2104,55 +2137,47 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="36" x14ac:dyDescent="0.15">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="144" x14ac:dyDescent="0.15">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="144" x14ac:dyDescent="0.15">
-      <c r="A10" s="25" t="s">
+      <c r="G9" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="156" x14ac:dyDescent="0.15">
+      <c r="A10" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="7" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Creacion de tablas para interfaces y tablas internas
</commit_message>
<xml_diff>
--- a/Analisis/Interfaces/interfaces.xlsx
+++ b/Analisis/Interfaces/interfaces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/Analisis/Interfaces/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="453" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30857D36-F44A-4CB9-BA74-960D0B4FB221}"/>
+  <xr:revisionPtr revIDLastSave="458" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{156F7DF3-3444-4C7B-9FF0-14A831F1AF20}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resumen" sheetId="2" r:id="rId1"/>
@@ -89,51 +89,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Las entidades podran enviar la codificacion oficial, es decir:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t xml:space="preserve">1: Si, deuda positiva
-2: Si, dedau negativa
-3: Si, deuda positiva y negativa
-4: No
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t xml:space="preserve">
-En caso que no, deberan relacionar el codigo de la entidad para determinar este concepto en la tabla "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t>operacion_titulo_rel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t xml:space="preserve">" </t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Se debe relacionar este codigo con la tabla interna "</t>
     </r>
     <r>
@@ -241,9 +196,6 @@
   </si>
   <si>
     <t>cod_tipo_obligacion</t>
-  </si>
-  <si>
-    <t>codigo de la entidad para determinar el concepto de la TABLA 126 del MSI de bancos que requiere REDEC</t>
   </si>
   <si>
     <t>tabla_banco_126_rel</t>
@@ -709,6 +661,55 @@
   </si>
   <si>
     <t>Corresponde al valor de la cuenta contable reportada expresado por su equivalente en pesos a la fecha de referencia del archivo, cuando se trate de operaciones reajustables o en moneda extranjera.</t>
+  </si>
+  <si>
+    <t>codigo de la entidad para determinar el concepto de la TABLA 126 del MSI de bancos que requiere REDEC.
+Aqui las entidades pueden enviar un codigo de producto o el mismo codigo de la tabla 126.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Las entidades podran enviar la codificacion oficial, es decir:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t xml:space="preserve">1: Si, deuda positiva
+2: Si, deuda negativa
+3: Si, deuda positiva y negativa
+4: No
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t xml:space="preserve">
+En caso que no, deberan relacionar el codigo de la entidad para determinar este concepto en la tabla "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>operacion_titulo_rel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t xml:space="preserve">" </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1160,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1192,33 +1193,33 @@
         <v>10</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="48" x14ac:dyDescent="0.15">
@@ -1235,10 +1236,10 @@
         <v>6</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="144" x14ac:dyDescent="0.15">
@@ -1249,7 +1250,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
@@ -1258,10 +1259,10 @@
         <v>15</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.15">
@@ -1275,10 +1276,10 @@
         <v>6</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="144" x14ac:dyDescent="0.15">
@@ -1289,7 +1290,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>19</v>
+        <v>117</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>6</v>
@@ -1298,10 +1299,10 @@
         <v>16</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="132" x14ac:dyDescent="0.15">
@@ -1312,317 +1313,317 @@
         <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="228" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8" ht="96" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="216" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="276" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="84" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="96" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="36" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="36" x14ac:dyDescent="0.15">
       <c r="A18" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A20" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A21" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="36" x14ac:dyDescent="0.15">
       <c r="A22" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="48" x14ac:dyDescent="0.15">
       <c r="A23" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D23" s="22" t="s">
         <v>6</v>
@@ -1630,59 +1631,59 @@
       <c r="E23" s="22"/>
       <c r="F23" s="23"/>
       <c r="G23" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H23" s="23"/>
     </row>
     <row r="24" spans="1:8" ht="48" x14ac:dyDescent="0.15">
       <c r="A24" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E24" s="22"/>
       <c r="F24" s="23"/>
       <c r="G24" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H24" s="23"/>
     </row>
     <row r="25" spans="1:8" ht="48" x14ac:dyDescent="0.15">
       <c r="A25" s="19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B25" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="21" t="s">
-        <v>99</v>
-      </c>
       <c r="D25" s="22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="23"/>
       <c r="G25" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H25" s="23"/>
     </row>
     <row r="26" spans="1:8" ht="144" x14ac:dyDescent="0.15">
       <c r="A26" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="21" t="s">
         <v>98</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>100</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>6</v>
@@ -1690,19 +1691,19 @@
       <c r="E26" s="22"/>
       <c r="F26" s="23"/>
       <c r="G26" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H26" s="23"/>
     </row>
     <row r="27" spans="1:8" ht="144" x14ac:dyDescent="0.15">
       <c r="A27" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="21" t="s">
         <v>102</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>104</v>
       </c>
       <c r="D27" s="22" t="s">
         <v>6</v>
@@ -1710,25 +1711,25 @@
       <c r="E27" s="22"/>
       <c r="F27" s="23"/>
       <c r="G27" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H27" s="23"/>
     </row>
     <row r="28" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>116</v>
-      </c>
       <c r="D28" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1741,7 +1742,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1772,21 +1773,21 @@
         <v>10</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="24" x14ac:dyDescent="0.15">
@@ -1800,125 +1801,125 @@
         <v>6</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="36" x14ac:dyDescent="0.15">
       <c r="A4" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A6" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A8" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A9" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A10" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A11" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1931,7 +1932,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1963,23 +1964,23 @@
     </row>
     <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -1987,13 +1988,13 @@
     </row>
     <row r="4" spans="1:5" ht="24" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2005,8 +2006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30384B7-8E23-4C8B-825F-E2F77541013E}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2037,38 +2038,38 @@
         <v>10</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.15">
+      <c r="A3" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>88</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.15">
@@ -2082,103 +2083,103 @@
         <v>6</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="84" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="36" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>109</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="36" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="144" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="156" x14ac:dyDescent="0.15">
       <c r="A10" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creacion de Dockerfile e instaladores para windows y linux- Airflow
</commit_message>
<xml_diff>
--- a/Analisis/Interfaces/interfaces.xlsx
+++ b/Analisis/Interfaces/interfaces.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="458" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{156F7DF3-3444-4C7B-9FF0-14A831F1AF20}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13590" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resumen" sheetId="2" r:id="rId1"/>
@@ -19,10 +19,21 @@
     <sheet name="tipo_cambio" sheetId="4" r:id="rId4"/>
     <sheet name="cuadro_rectificaciones" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2006,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30384B7-8E23-4C8B-825F-E2F77541013E}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2058,7 +2069,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
Correccion campo fecha_aceleracion, tenia que estar como date, correccion DAG para importar interfaz
</commit_message>
<xml_diff>
--- a/Analisis/Interfaces/interfaces.xlsx
+++ b/Analisis/Interfaces/interfaces.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/Analisis/Interfaces/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="458" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{156F7DF3-3444-4C7B-9FF0-14A831F1AF20}"/>
+  <xr:revisionPtr revIDLastSave="459" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E02041F8-04D6-45A7-9C4A-087FA461B2A3}"/>
   <bookViews>
-    <workbookView xWindow="13590" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resumen" sheetId="2" r:id="rId1"/>
@@ -1172,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1597,7 +1597,7 @@
         <v>80</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>31</v>
@@ -2017,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30384B7-8E23-4C8B-825F-E2F77541013E}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2069,7 +2069,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
Creacion de validacion interfaz cartera_operaciones, correccion tablas log
</commit_message>
<xml_diff>
--- a/Analisis/Interfaces/interfaces.xlsx
+++ b/Analisis/Interfaces/interfaces.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="459" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E02041F8-04D6-45A7-9C4A-087FA461B2A3}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resumen" sheetId="2" r:id="rId1"/>
@@ -1172,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1753,7 +1753,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2017,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30384B7-8E23-4C8B-825F-E2F77541013E}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection sqref="A1:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2069,7 +2069,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
Procedimientos val_interfaz_A01, val_interfaz_B01, trunca_tablas
</commit_message>
<xml_diff>
--- a/Analisis/Interfaces/interfaces.xlsx
+++ b/Analisis/Interfaces/interfaces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/Analisis/Interfaces/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="459" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E02041F8-04D6-45A7-9C4A-087FA461B2A3}"/>
+  <xr:revisionPtr revIDLastSave="462" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA64D172-F508-41C9-B856-96CB812AFD4E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resumen" sheetId="2" r:id="rId1"/>
@@ -1156,7 +1156,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1172,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1753,7 +1753,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2017,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30384B7-8E23-4C8B-825F-E2F77541013E}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection sqref="A1:G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Avance en procedimiento para RDC01
</commit_message>
<xml_diff>
--- a/Analisis/Interfaces/interfaces.xlsx
+++ b/Analisis/Interfaces/interfaces.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="462" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA64D172-F508-41C9-B856-96CB812AFD4E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resumen" sheetId="2" r:id="rId1"/>
@@ -1172,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2069,7 +2069,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
Avance en carga financiera, monto original, monto actual
</commit_message>
<xml_diff>
--- a/Analisis/Interfaces/interfaces.xlsx
+++ b/Analisis/Interfaces/interfaces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/Analisis/Interfaces/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="462" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA64D172-F508-41C9-B856-96CB812AFD4E}"/>
+  <xr:revisionPtr revIDLastSave="472" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AD35F06-639F-439B-ABDB-D7949E1C254E}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="121">
   <si>
     <t>Campo</t>
   </si>
@@ -267,9 +267,6 @@
   </si>
   <si>
     <t>numeric</t>
-  </si>
-  <si>
-    <t>Por analizar en mas detalle, se podria sacar desde el cuadro de pago.</t>
   </si>
   <si>
     <t>gar_real_inmobiliaria</t>
@@ -314,9 +311,6 @@
 Para operaciones del TIPO DE OBLIGACIÓN REPORTABLE de leasing con código 31, 32 o 33 del campo 6, este monto será completado con el monto remanente de la duración del contrato.</t>
   </si>
   <si>
-    <t>Informar en moneda de origen</t>
-  </si>
-  <si>
     <t>capital</t>
   </si>
   <si>
@@ -721,6 +715,23 @@
       </rPr>
       <t xml:space="preserve">" </t>
     </r>
+  </si>
+  <si>
+    <t>Informar el valor en pesos</t>
+  </si>
+  <si>
+    <t>Informar en moneda de origen
+Para el leasing tambien informar el monto original no el remanente, ya que el remanente se sacara desde el cuadro de pago.</t>
+  </si>
+  <si>
+    <t>Si existe la categoria otros y que este pagado, debe ir aca.</t>
+  </si>
+  <si>
+    <t>otros_pagado</t>
+  </si>
+  <si>
+    <t>Tiene sentido para tipos de obligaciones 07 y 08, usos de tarjetas de credito y uso de lineas de creditos.
+Para los otros tipos de obligacion no contingente, el valor a reportar en el RDC01 se sacara desde el cuadro de pago.</t>
   </si>
 </sst>
 </file>
@@ -1172,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1204,21 +1215,21 @@
         <v>10</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>26</v>
@@ -1301,7 +1312,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>6</v>
@@ -1344,7 +1355,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>24</v>
@@ -1390,7 +1401,7 @@
         <v>29</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>35</v>
+        <v>120</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>34</v>
@@ -1423,10 +1434,13 @@
     </row>
     <row r="12" spans="1:8" ht="216" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>37</v>
+      <c r="C12" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>34</v>
@@ -1440,10 +1454,13 @@
     </row>
     <row r="13" spans="1:8" ht="276" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>39</v>
+      <c r="C13" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>34</v>
@@ -1457,10 +1474,13 @@
     </row>
     <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>41</v>
+      <c r="C14" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>34</v>
@@ -1474,10 +1494,13 @@
     </row>
     <row r="15" spans="1:8" ht="84" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>43</v>
+      <c r="C15" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>34</v>
@@ -1491,13 +1514,13 @@
     </row>
     <row r="16" spans="1:8" ht="96" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="C16" s="4" t="s">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>34</v>
@@ -1511,13 +1534,13 @@
     </row>
     <row r="17" spans="1:8" ht="36" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>34</v>
@@ -1531,13 +1554,13 @@
     </row>
     <row r="18" spans="1:8" ht="36" x14ac:dyDescent="0.15">
       <c r="A18" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>34</v>
@@ -1551,13 +1574,13 @@
     </row>
     <row r="19" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>34</v>
@@ -1571,10 +1594,10 @@
     </row>
     <row r="20" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A20" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>6</v>
@@ -1588,13 +1611,13 @@
     </row>
     <row r="21" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A21" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>26</v>
@@ -1608,13 +1631,13 @@
     </row>
     <row r="22" spans="1:8" ht="36" x14ac:dyDescent="0.15">
       <c r="A22" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>6</v>
@@ -1628,13 +1651,13 @@
     </row>
     <row r="23" spans="1:8" ht="48" x14ac:dyDescent="0.15">
       <c r="A23" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D23" s="22" t="s">
         <v>6</v>
@@ -1648,13 +1671,13 @@
     </row>
     <row r="24" spans="1:8" ht="48" x14ac:dyDescent="0.15">
       <c r="A24" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D24" s="22" t="s">
         <v>26</v>
@@ -1668,13 +1691,13 @@
     </row>
     <row r="25" spans="1:8" ht="48" x14ac:dyDescent="0.15">
       <c r="A25" s="19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B25" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="21" t="s">
         <v>95</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>97</v>
       </c>
       <c r="D25" s="22" t="s">
         <v>26</v>
@@ -1688,13 +1711,13 @@
     </row>
     <row r="26" spans="1:8" ht="144" x14ac:dyDescent="0.15">
       <c r="A26" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="21" t="s">
         <v>96</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>98</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>6</v>
@@ -1708,13 +1731,13 @@
     </row>
     <row r="27" spans="1:8" ht="144" x14ac:dyDescent="0.15">
       <c r="A27" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="21" t="s">
         <v>100</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>102</v>
       </c>
       <c r="D27" s="22" t="s">
         <v>6</v>
@@ -1728,13 +1751,13 @@
     </row>
     <row r="28" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>114</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>34</v>
@@ -1750,10 +1773,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCCEABFF-C145-4CD4-8906-0ADE13F77864}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1789,10 +1812,10 @@
     </row>
     <row r="2" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>26</v>
@@ -1817,13 +1840,13 @@
     </row>
     <row r="4" spans="1:6" ht="36" x14ac:dyDescent="0.15">
       <c r="A4" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>26</v>
@@ -1834,10 +1857,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>34</v>
@@ -1848,10 +1871,10 @@
     </row>
     <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A6" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>34</v>
@@ -1862,10 +1885,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>34</v>
@@ -1876,10 +1899,10 @@
     </row>
     <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A8" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>34</v>
@@ -1890,10 +1913,10 @@
     </row>
     <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A9" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>34</v>
@@ -1904,10 +1927,10 @@
     </row>
     <row r="10" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A10" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>34</v>
@@ -1918,18 +1941,35 @@
     </row>
     <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A11" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F11" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="A12" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1975,10 +2015,10 @@
     </row>
     <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="3" t="s">
@@ -1988,10 +2028,10 @@
     </row>
     <row r="3" spans="1:5" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -1999,10 +2039,10 @@
     </row>
     <row r="4" spans="1:5" ht="24" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>34</v>
@@ -2052,15 +2092,15 @@
         <v>30</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>26</v>
@@ -2071,10 +2111,10 @@
     </row>
     <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>26</v>
@@ -2099,13 +2139,13 @@
     </row>
     <row r="5" spans="1:7" ht="84" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>34</v>
@@ -2116,13 +2156,13 @@
     </row>
     <row r="6" spans="1:7" ht="36" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>34</v>
@@ -2133,13 +2173,13 @@
     </row>
     <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>6</v>
@@ -2150,10 +2190,10 @@
     </row>
     <row r="8" spans="1:7" ht="36" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>26</v>
@@ -2164,10 +2204,10 @@
     </row>
     <row r="9" spans="1:7" ht="144" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>34</v>
@@ -2178,13 +2218,13 @@
     </row>
     <row r="10" spans="1:7" ht="156" x14ac:dyDescent="0.15">
       <c r="A10" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Incorporacion de interface de garantias
</commit_message>
<xml_diff>
--- a/Analisis/Interfaces/interfaces.xlsx
+++ b/Analisis/Interfaces/interfaces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/Analisis/Interfaces/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="472" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AD35F06-639F-439B-ABDB-D7949E1C254E}"/>
+  <xr:revisionPtr revIDLastSave="531" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64AA1F5C-D56A-42A1-A668-83BFB8DABB17}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15210" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resumen" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="cuadro_operaciones" sheetId="5" r:id="rId3"/>
     <sheet name="tipo_cambio" sheetId="4" r:id="rId4"/>
     <sheet name="cuadro_rectificaciones" sheetId="6" r:id="rId5"/>
+    <sheet name="cartera_garantias" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="133">
   <si>
     <t>Campo</t>
   </si>
@@ -91,12 +92,6 @@
   </si>
   <si>
     <t>operacion_titulo_rel</t>
-  </si>
-  <si>
-    <t>cod_deudor</t>
-  </si>
-  <si>
-    <t>codigo de la entidad para poder identificar el tipo de deudor que requiere el MSI.</t>
   </si>
   <si>
     <r>
@@ -156,53 +151,6 @@
       </rPr>
       <t xml:space="preserve">
 Esto quiere decir que si la entidad envia 1 o 2 no tendra que realizar la realicacion con la tabla interna para determinar este campo.</t>
-    </r>
-  </si>
-  <si>
-    <t>tipo_deudor_rel</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Las entidades podran enviar la codificacion oficial, es decir:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t xml:space="preserve">1: Deudor directo
-2: Deudor indirecto
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t xml:space="preserve">
-En caso que no, deberan relacionar el codigo de la entidad para determinar este concepto en la tabla "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t>tipo_deudor_rel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t xml:space="preserve">"
-</t>
     </r>
   </si>
   <si>
@@ -272,25 +220,9 @@
     <t>gar_real_inmobiliaria</t>
   </si>
   <si>
-    <t>Corresponde al valor total de las garantías inmobiliarias constituidas para la operación reportada disponible en la fecha de referencia del archivo. En este campo se debe informar la tasación comercial, de acuerdo con el marco regulatorio aplicable a la respectiva entidad reportante. En caso de no contar con lo anterior, se deberá considerar la tasación fiscal. A falta de las tasaciones anteriores, se deberá reportar un valor de acuerdo con las metodologías o políticas internas que tenga la entidad reportante. Cuando todo lo anterior no sea posible, se deberá reportar valor cero.
-Las garantías en moneda extranjera o en pesos reajustables, se informarán actualizadas al tipo de cambio de representación contable o valor de la unidad reajustable al último día del mes de referencia de la información.
-En el caso de que la garantía sea general, la entidad reportante deberá realizar una razonable estimación del valor que se le asociaría a la obligación reportable, y ser informada en este campo. La suma de las estimaciones para todas las obligaciones reportables garantizadas por la misma garantía general debe ser consistente con su valor.</t>
-  </si>
-  <si>
     <t>gar_real_mobiliaria</t>
   </si>
   <si>
-    <t>Corresponde al valor total de las garantías constituidas en bienes muebles para la operación reportada disponible en la fecha de referencia del archivo. En este campo se debe informar
-Manual del Sistema de Información para REDEC
-Sistema de Reportantes
-ARCHIVO RDC01
-Hoja 5
-Oficio Circular N°1.387 / 02.10.2025
-la tasación comercial, de acuerdo con el marco regulatorio aplicable a la respectiva entidad reportante. En caso de no contar con lo anterior, se deberá considerar la tasación fiscal. A falta de las tasaciones anteriores, se deberá reportar un valor de acuerdo con las metodologías o políticas internas que tenga la entidad reportante. Cuando todo lo anterior no sea posible, se deberá reportar valor cero.
-Las garantías en moneda extranjera o en pesos reajustables, se informarán actualizadas al tipo de cambio de representación contable o valor de la unidad reajustable al último día del mes de referencia de la información.
-En el caso de que la garantía sea general, la entidad reportante deberá realizar una razonable estimación del valor que se le asociaría a la obligación reportable, y ser informada en este campo. La suma de las estimaciones para todas las obligaciones reportables garantizadas por la misma garantía general debe ser consistente con su valor.</t>
-  </si>
-  <si>
     <t>gar_financiera</t>
   </si>
   <si>
@@ -298,9 +230,6 @@
   </si>
   <si>
     <t>gar_personal</t>
-  </si>
-  <si>
-    <t>Se informará el monto avalado o afianzado y valorado en pesos a la fecha origen de aquella garantía a favor del reportante consignada en un contrato firmado o certificado por la persona que otorga la garantía. Cuando el límite de la garantía sea “ilimitado”, corresponde incluir el monto total de los créditos cubiertos al momento de la constitución de esa garantía. En el evento de que no se disponga de ese valor, el campo se informará con cero.</t>
   </si>
   <si>
     <t>monto_original</t>
@@ -732,6 +661,83 @@
   <si>
     <t>Tiene sentido para tipos de obligaciones 07 y 08, usos de tarjetas de credito y uso de lineas de creditos.
 Para los otros tipos de obligacion no contingente, el valor a reportar en el RDC01 se sacara desde el cuadro de pago.</t>
+  </si>
+  <si>
+    <t>id_garantia</t>
+  </si>
+  <si>
+    <t>Codigo que identifica de manera unica a la garantia.</t>
+  </si>
+  <si>
+    <t>rut_garante</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>Corresponde al RUT del deudor indirecto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>. En caso de tratarse de una persona, ya sea natural o jurídica, que no posea RUT, se debe informar el “RUT ficticio” asignado, de acuerdo con las instrucciones generales del MSI REDEC.</t>
+    </r>
+  </si>
+  <si>
+    <t>codigo de la Entidad Financiera para identificar que tipo de cliente es el garante, por ejemplo: Personal Natural, Persona Juridica</t>
+  </si>
+  <si>
+    <t>Corresponde al código que identifica en forma unívoca a la operación de crédito que esta garantizando</t>
+  </si>
+  <si>
+    <t>En este campo se debe informar la tasación comercial, de acuerdo con el marco regulatorio aplicable a la respectiva entidad reportante. En caso de no contar con lo anterior, se deberá considerar la tasación fiscal. A falta de las tasaciones anteriores, se deberá reportar un valor de acuerdo con las metodologías o políticas internas que tenga la entidad reportante. Cuando todo lo anterior no sea posible, se deberá reportar valor cero.
+Las garantías en moneda extranjera o en pesos reajustables, se informarán actualizadas al tipo de cambio de representación contable o valor de la unidad reajustable al último día del mes de referencia de la información.
+En el caso de que la garantía sea general, la entidad reportante deberá realizar una razonable estimación del valor que se le asociaría a la obligación reportable, y ser informada en este campo. La suma de las estimaciones para todas las obligaciones reportables garantizadas por la misma garantía general debe ser consistente con su valor.</t>
+  </si>
+  <si>
+    <t>Corresponde a la fecha (AAAAMMDD) de otorgamiento original de la garantia</t>
+  </si>
+  <si>
+    <t>porc_real_inmobiliaria</t>
+  </si>
+  <si>
+    <t>Porcentaje de la garantia real inmobiliaria que cubre la operacion.</t>
+  </si>
+  <si>
+    <t>Ejemplo: 100% informar 100</t>
+  </si>
+  <si>
+    <t>En este campo se debe informar la tasación comercial, de acuerdo con el marco regulatorio aplicable a la respectiva entidad reportante. En caso de no contar con lo anterior, se deberá considerar la tasación fiscal. A falta de las tasaciones anteriores, se deberá reportar un valor de acuerdo con las metodologías o políticas internas que tenga la entidad reportante. Cuando todo lo anterior no sea posible, se deberá reportar valor cero.
+Las garantías en moneda extranjera o en pesos reajustables, se informarán actualizadas al tipo de cambio de representación contable o valor de la unidad reajustable al último día del mes de referencia de la información.
+En el caso de que la garantía sea general, la entidad reportante deberá realizar una razonable estimación del valor que se le asociaría a la obligación reportable, y ser informada en este campo.</t>
+  </si>
+  <si>
+    <t>porc_real_mobiliaria</t>
+  </si>
+  <si>
+    <t>Porcentaje de la garantia real mobiliaria que cubre la operacion.</t>
+  </si>
+  <si>
+    <t>porc_financiera</t>
+  </si>
+  <si>
+    <t>Porcentaje de la garantia financiera que cubre la operacion.</t>
+  </si>
+  <si>
+    <t>porc_personal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se informará el monto avalado o afianzado y valorado en pesos a la fecha origen de aquella garantía a favor del reportante consignada en un contrato firmado o certificado por la persona que otorga la garantía. </t>
+  </si>
+  <si>
+    <t>Porcentaje de la garantia personal que cubre la operacion.</t>
   </si>
 </sst>
 </file>
@@ -1181,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1215,33 +1221,33 @@
         <v>10</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="48" x14ac:dyDescent="0.15">
@@ -1258,10 +1264,10 @@
         <v>6</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="144" x14ac:dyDescent="0.15">
@@ -1272,7 +1278,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
@@ -1281,10 +1287,10 @@
         <v>15</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.15">
@@ -1298,10 +1304,10 @@
         <v>6</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="144" x14ac:dyDescent="0.15">
@@ -1312,7 +1318,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>6</v>
@@ -1321,449 +1327,346 @@
         <v>16</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="132" x14ac:dyDescent="0.15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>18</v>
+        <v>107</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.15">
+        <v>27</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="F8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="228" x14ac:dyDescent="0.15">
+      <c r="A9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A9" s="17" t="s">
+      <c r="B9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="228" x14ac:dyDescent="0.15">
-      <c r="A10" s="18" t="s">
+      <c r="C9" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:8" ht="96" x14ac:dyDescent="0.15">
+      <c r="A10" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="10"/>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="96" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="216" x14ac:dyDescent="0.15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="36" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>116</v>
+        <v>52</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="276" x14ac:dyDescent="0.15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="36" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>116</v>
+        <v>51</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>116</v>
+        <v>50</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="84" x14ac:dyDescent="0.15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>116</v>
+        <v>43</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="96" x14ac:dyDescent="0.15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>117</v>
+        <v>71</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="36" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>47</v>
+        <v>73</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="36" x14ac:dyDescent="0.15">
-      <c r="A18" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A19" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A20" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="48" x14ac:dyDescent="0.15">
+      <c r="A18" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
+      <c r="E18" s="22"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" s="23"/>
+    </row>
+    <row r="19" spans="1:8" ht="48" x14ac:dyDescent="0.15">
+      <c r="A19" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="36" x14ac:dyDescent="0.15">
-      <c r="A22" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="B19" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="22"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="23"/>
+    </row>
+    <row r="20" spans="1:8" ht="48" x14ac:dyDescent="0.15">
+      <c r="A20" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="22"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="23"/>
+    </row>
+    <row r="21" spans="1:8" ht="144" x14ac:dyDescent="0.15">
+      <c r="A21" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="48" x14ac:dyDescent="0.15">
-      <c r="A23" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B23" s="20" t="s">
+      <c r="E21" s="22"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="23"/>
+    </row>
+    <row r="22" spans="1:8" ht="144" x14ac:dyDescent="0.15">
+      <c r="A22" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="22" t="s">
+      <c r="B22" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" s="23"/>
-    </row>
-    <row r="24" spans="1:8" ht="48" x14ac:dyDescent="0.15">
-      <c r="A24" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="22"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" s="23"/>
-    </row>
-    <row r="25" spans="1:8" ht="48" x14ac:dyDescent="0.15">
-      <c r="A25" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="22"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H25" s="23"/>
-    </row>
-    <row r="26" spans="1:8" ht="144" x14ac:dyDescent="0.15">
-      <c r="A26" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="22"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H26" s="23"/>
-    </row>
-    <row r="27" spans="1:8" ht="144" x14ac:dyDescent="0.15">
-      <c r="A27" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" s="22"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H27" s="23"/>
-    </row>
-    <row r="28" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>31</v>
+      <c r="E22" s="22"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" s="23"/>
+    </row>
+    <row r="23" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1807,21 +1710,21 @@
         <v>10</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="24" x14ac:dyDescent="0.15">
@@ -1835,142 +1738,142 @@
         <v>6</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="36" x14ac:dyDescent="0.15">
       <c r="A4" s="15" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="15" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A6" s="15" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="15" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A8" s="15" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A9" s="15" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A10" s="15" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A11" s="15" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2015,23 +1918,23 @@
     </row>
     <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -2039,13 +1942,13 @@
     </row>
     <row r="4" spans="1:5" ht="24" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2057,7 +1960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30384B7-8E23-4C8B-825F-E2F77541013E}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -2089,38 +1992,38 @@
         <v>10</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.15">
@@ -2134,103 +2037,382 @@
         <v>6</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="84" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="36" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="36" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="144" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="156" x14ac:dyDescent="0.15">
       <c r="A10" s="17" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0031ED8-A2FE-4866-A880-33D709C0EF55}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="7.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.15">
+      <c r="A2" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="48" x14ac:dyDescent="0.15">
+      <c r="A4" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="156" x14ac:dyDescent="0.15">
+      <c r="A5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="24" x14ac:dyDescent="0.15">
+      <c r="A6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="24" x14ac:dyDescent="0.15">
+      <c r="A7" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="192" x14ac:dyDescent="0.15">
+      <c r="A8" s="17" t="s">
         <v>31</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="168" x14ac:dyDescent="0.15">
+      <c r="A10" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.15">
+      <c r="A12" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="48" x14ac:dyDescent="0.15">
+      <c r="A14" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Avance en ajuste de diferencias cuando garantia es menor al monto actual
</commit_message>
<xml_diff>
--- a/Analisis/Interfaces/interfaces.xlsx
+++ b/Analisis/Interfaces/interfaces.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="531" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64AA1F5C-D56A-42A1-A668-83BFB8DABB17}"/>
   <bookViews>
-    <workbookView xWindow="-15210" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resumen" sheetId="2" r:id="rId1"/>
@@ -2145,9 +2145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0031ED8-A2FE-4866-A880-33D709C0EF55}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>